<commit_message>
Added mandatory pan for entity and investor
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_investors.xlsx
+++ b/public/sample_uploads/fund_investors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4919C6AC-2B8F-4EC5-9EB2-2B4C1429C2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D06D1E-0370-4696-A58D-4717422D7DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="2880" windowWidth="18000" windowHeight="10433" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Investors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Tags</t>
   </si>
@@ -95,6 +95,27 @@
   </si>
   <si>
     <t>Investor 6</t>
+  </si>
+  <si>
+    <t>PAN *</t>
+  </si>
+  <si>
+    <t>BUHNXDFEA6</t>
+  </si>
+  <si>
+    <t>JN2GOV5FYI</t>
+  </si>
+  <si>
+    <t>CGKT9ROWB1</t>
+  </si>
+  <si>
+    <t>4I3FNDATK0</t>
+  </si>
+  <si>
+    <t>5AM81UTOQB</t>
+  </si>
+  <si>
+    <t>QNEL3S7Z2J</t>
   </si>
 </sst>
 </file>
@@ -141,10 +162,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,144 +484,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="18.06640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="1" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="18.06640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="D9" s="1"/>
+    <row r="8" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="3"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="3"/>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Investor email ex pan (#158)
* Added esign_emails to kyc and commitment

* Added tests for import esign_emails

* No longer use fund_signatory and trustee_signatory

* Fixed misc bugs

* Added header custom field

* Added DataList to custom field types

* Added RansackerAmounts

* Now filters work on dollars and not cents

* Simplified commitment imports, need to test bulk upload

* Added agreement_amount to kyc

* Added validations and uniq index to FCF names

* Added has_scopes to kyc controller

* Added agreement_overcalled to kyc

* Handle dup FCF names

* Added is_fund? to enable Angel Funds
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_investors.xlsx
+++ b/public/sample_uploads/fund_investors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D06D1E-0370-4696-A58D-4717422D7DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61CF8D7-F5E3-4CFC-B760-2BA564C9F38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2880" windowWidth="18000" windowHeight="10433" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Investors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Tags</t>
   </si>
@@ -116,6 +116,27 @@
   </si>
   <si>
     <t>QNEL3S7Z2J</t>
+  </si>
+  <si>
+    <t>Primary Email</t>
+  </si>
+  <si>
+    <t>emp1@gmail.com</t>
+  </si>
+  <si>
+    <t>emp2@gmail.com</t>
+  </si>
+  <si>
+    <t>emp3@gmail.com</t>
+  </si>
+  <si>
+    <t>emp4@gmail.com</t>
+  </si>
+  <si>
+    <t>emp5@gmail.com</t>
+  </si>
+  <si>
+    <t>emp6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -162,12 +183,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,25 +503,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E1" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="18.06640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -512,17 +531,20 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -532,17 +554,20 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -552,17 +577,20 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -572,17 +600,20 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -592,17 +623,20 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -612,17 +646,20 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
@@ -631,20 +668,21 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-      <c r="E9" s="1"/>
+    <row r="8" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>